<commit_message>
August Op Plan deliverable done
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019_AM.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 07_31_2019/Offsets and Clip times 07_31_2019_AM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9336" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Offsets" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -472,6 +472,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +512,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -854,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2724,11 +2727,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFC1360"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B320" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B164" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A319" sqref="A319:XFD323"/>
+      <selection pane="bottomRight" activeCell="A176" sqref="A176:XFD180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20027,159 +20030,158 @@
         <v>47</v>
       </c>
     </row>
-    <row r="349" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A349" s="3" t="s">
+    <row r="349" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A349" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B349" s="8">
+      <c r="B349" s="33">
         <v>43591.375</v>
       </c>
-      <c r="C349" s="8">
+      <c r="C349" s="33">
         <v>43592.458333333336</v>
       </c>
-      <c r="D349" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="350" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A350" s="3" t="s">
+      <c r="D349" s="34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A350" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B350" s="8">
+      <c r="B350" s="33">
         <v>43592.125</v>
       </c>
-      <c r="C350" s="8">
+      <c r="C350" s="33">
         <v>43594.416666666664</v>
       </c>
-      <c r="D350" s="7" t="s">
+      <c r="D350" s="34" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A351" s="3" t="s">
+    <row r="351" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A351" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B351" s="8">
+      <c r="B351" s="33">
         <v>43595.291666666664</v>
       </c>
-      <c r="C351" s="8">
+      <c r="C351" s="33">
         <v>43595.416666666664</v>
       </c>
-      <c r="D351" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E351" s="7"/>
-    </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A352" s="3" t="s">
+      <c r="D351" s="34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A352" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B352" s="8">
+      <c r="B352" s="33">
         <v>43596.319444444445</v>
       </c>
-      <c r="C352" s="8">
+      <c r="C352" s="33">
         <v>43596.947916666664</v>
       </c>
-      <c r="D352" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A353" s="3" t="s">
+      <c r="D352" s="34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A353" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B353" s="8">
+      <c r="B353" s="33">
         <v>43601.333333333336</v>
       </c>
-      <c r="C353" s="8">
+      <c r="C353" s="33">
         <v>43601.854166666664</v>
       </c>
-      <c r="D353" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E353" s="3"/>
-    </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A354" s="3" t="s">
+      <c r="D353" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E353" s="32"/>
+    </row>
+    <row r="354" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A354" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B354" s="8">
+      <c r="B354" s="33">
         <v>43604.083333333336</v>
       </c>
-      <c r="C354" s="8">
+      <c r="C354" s="33">
         <v>43605.1875</v>
       </c>
-      <c r="D354" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A355" s="3" t="s">
+      <c r="D354" s="34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A355" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B355" s="8">
+      <c r="B355" s="33">
         <v>43604.083333333336</v>
       </c>
-      <c r="C355" s="8">
+      <c r="C355" s="33">
         <v>43633.6875</v>
       </c>
-      <c r="D355" s="7" t="s">
+      <c r="D355" s="34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A356" s="3" t="s">
+    <row r="356" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A356" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B356" s="8">
+      <c r="B356" s="33">
         <v>43637.270833333336</v>
       </c>
-      <c r="C356" s="8">
+      <c r="C356" s="33">
         <v>43637.479166666664</v>
       </c>
-      <c r="D356" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="357" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A357" s="3" t="s">
+      <c r="D356" s="34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A357" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B357" s="8">
+      <c r="B357" s="33">
         <v>43663.302083333336</v>
       </c>
-      <c r="C357" s="8">
+      <c r="C357" s="33">
         <v>43665.5625</v>
       </c>
-      <c r="D357" s="7" t="s">
+      <c r="D357" s="34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="358" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A358" s="8" t="s">
+    <row r="358" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A358" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B358" s="8">
+      <c r="B358" s="33">
         <v>43668.850694444445</v>
       </c>
-      <c r="C358" s="8">
+      <c r="C358" s="33">
         <v>43669.267361111109</v>
       </c>
-      <c r="D358" s="7" t="s">
+      <c r="D358" s="34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="359" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A359" s="8" t="s">
+    <row r="359" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A359" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B359" s="8">
+      <c r="B359" s="33">
         <v>43675.892361111109</v>
       </c>
-      <c r="C359" s="8">
+      <c r="C359" s="33">
         <v>43676.225694444445</v>
       </c>
-      <c r="D359" s="7" t="s">
+      <c r="D359" s="34" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>